<commit_message>
Experiment with Excel Labs
</commit_message>
<xml_diff>
--- a/CH-57 Fuzzy Numbers Calculation.xlsx
+++ b/CH-57 Fuzzy Numbers Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E4C7C8-FDC8-4423-A497-7453AF03ACF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3000AB37-DAAE-47BA-A8AA-37BFF465FB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
   <definedNames>
     <definedName name="_nA">SingleFunction!$B$3:$B$15</definedName>
     <definedName name="_nB">SingleFunction!$C$3:$C$15</definedName>
+    <definedName name="Test" comment="Test">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a + _xlpm.b)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +44,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -55,16 +57,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="57">
   <si>
     <t>Result</t>
   </si>
@@ -229,6 +245,12 @@
   </si>
   <si>
     <t>Dif</t>
+  </si>
+  <si>
+    <t>Let's experiment with Excel Labs</t>
+  </si>
+  <si>
+    <t>Can I make a comment?</t>
   </si>
 </sst>
 </file>
@@ -264,7 +286,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,6 +302,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -376,12 +404,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,6 +746,64 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>7</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Berlin">
   <a:themeElements>
@@ -971,6 +1058,35 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="612" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9BD65D3B-C62F-495F-837A-780821296A8D}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{DCDCC851-1F35-45AF-8C7D-B5B9C789E9AA}&quot;}"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
@@ -993,14 +1109,14 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1295,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29732F5-A470-44B9-AC68-6F7D53F9D0BF}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1313,14 +1429,14 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1950,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA82B75F-2C8A-4884-B44A-F70DA9CCAD71}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1965,18 +2081,21 @@
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="G1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" s="12"/>
+      <c r="K1" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
@@ -1992,8 +2111,11 @@
         <v>27</v>
       </c>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
@@ -2010,7 +2132,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -2027,7 +2149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -2044,7 +2166,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -2061,7 +2183,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6" t="s">
         <v>10</v>
@@ -2078,7 +2200,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
@@ -2094,7 +2216,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
@@ -2110,7 +2232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
@@ -2126,7 +2248,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
@@ -2142,7 +2264,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>20</v>
       </c>
@@ -2159,7 +2281,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
@@ -2176,7 +2298,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2193,7 +2315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
@@ -2210,22 +2332,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="4:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="str" cm="1">
         <f t="array" ref="E19:F32">_xlfn.LET(
@@ -2244,9 +2366,12 @@
       <c r="F19" s="8" t="str">
         <v>A-B</v>
       </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="11"/>
+      <c r="K19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D20" s="3"/>
       <c r="E20" s="6" t="str">
         <v>5,8,14</v>
@@ -2254,7 +2379,7 @@
       <c r="F20" s="6" t="str">
         <v>-2,2,7</v>
       </c>
-      <c r="G20" s="12"/>
+      <c r="G20" s="11"/>
       <c r="H20" t="b" cm="1">
         <f t="array" ref="H20:I32">E20:F32=G3:H15</f>
         <v>1</v>
@@ -2263,29 +2388,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E21" s="6" t="str">
         <v>6,17,19</v>
       </c>
       <c r="F21" s="6" t="str">
         <v>-7,3,6</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="11"/>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E22" s="6" t="str">
         <v>4,6,10</v>
       </c>
       <c r="F22" s="6" t="str">
         <v>-3,0,3</v>
       </c>
-      <c r="G22" s="12"/>
+      <c r="G22" s="11"/>
       <c r="H22" t="b">
         <v>1</v>
       </c>
@@ -2293,14 +2421,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E23" s="6" t="str">
         <v>4,13,19</v>
       </c>
       <c r="F23" s="6" t="str">
         <v>-7,1,8</v>
       </c>
-      <c r="G23" s="12"/>
+      <c r="G23" s="11"/>
       <c r="H23" t="b">
         <v>1</v>
       </c>
@@ -2308,14 +2436,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E24" s="6" t="str">
         <v>11,14,20</v>
       </c>
       <c r="F24" s="6" t="str">
         <v>-5,-4,4</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="11"/>
       <c r="H24" t="b">
         <v>1</v>
       </c>
@@ -2323,44 +2451,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E25" s="6" t="str">
         <v>10,12,16</v>
       </c>
       <c r="F25" s="6" t="str">
         <v>0,2,6</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="11"/>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="K25" s="13" t="e" cm="1" vm="1">
+        <f t="array" ref="K25">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, _xlpm.a + _xlpm.b)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E26" s="6" t="str">
         <v>4,6,14</v>
       </c>
       <c r="F26" s="6" t="str">
         <v>-7,2,3</v>
       </c>
-      <c r="G26" s="12"/>
+      <c r="G26" s="11"/>
       <c r="H26" t="b">
         <v>1</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="K26" cm="1">
+        <f t="array" ref="K26">Test(K1,J2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E27" s="6" t="str">
         <v>3,8,17</v>
       </c>
       <c r="F27" s="6" t="str">
         <v>-7,0,7</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="G27" s="11"/>
       <c r="H27" t="b">
         <v>1</v>
       </c>
@@ -2368,14 +2504,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E28" s="6" t="str">
         <v>11,15,18</v>
       </c>
       <c r="F28" s="6" t="str">
         <v>-3,-1,4</v>
       </c>
-      <c r="G28" s="12"/>
+      <c r="G28" s="11"/>
       <c r="H28" t="b">
         <v>1</v>
       </c>
@@ -2383,14 +2519,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E29" s="6" t="str">
         <v>5,11,16</v>
       </c>
       <c r="F29" s="6" t="str">
         <v>-3,-1,8</v>
       </c>
-      <c r="G29" s="12"/>
+      <c r="G29" s="11"/>
       <c r="H29" t="b">
         <v>1</v>
       </c>
@@ -2398,14 +2534,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E30" s="6" t="str">
         <v>9,15,18</v>
       </c>
       <c r="F30" s="6" t="str">
         <v>-5,-1,4</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="11"/>
       <c r="H30" t="b">
         <v>1</v>
       </c>
@@ -2413,14 +2549,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E31" s="6" t="str">
         <v>11,14,20</v>
       </c>
       <c r="F31" s="6" t="str">
         <v>-5,-2,4</v>
       </c>
-      <c r="G31" s="12"/>
+      <c r="G31" s="11"/>
       <c r="H31" t="b">
         <v>1</v>
       </c>
@@ -2428,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E32" s="6" t="str">
         <v>6,14,18</v>
       </c>
@@ -2450,4 +2586,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAE0ARABZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCDCC851-1F35-45AF-8C7D-B5B9C789E9AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Play with Excel Labs
</commit_message>
<xml_diff>
--- a/CH-57 Fuzzy Numbers Calculation.xlsx
+++ b/CH-57 Fuzzy Numbers Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3000AB37-DAAE-47BA-A8AA-37BFF465FB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461EE71E-7721-48F6-8931-0A0BFDC74F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,8 @@
   <definedNames>
     <definedName name="_nA">SingleFunction!$B$3:$B$15</definedName>
     <definedName name="_nB">SingleFunction!$C$3:$C$15</definedName>
+    <definedName name="FunctionOutput" comment="Area where I do my testing">SingleFunction!$E$20:$F$32</definedName>
+    <definedName name="Rubric" comment="Desired Output">SingleFunction!$G$3:$H$15</definedName>
     <definedName name="Test" comment="Test">_xlfn.LAMBDA(_xlpm.a,_xlpm.b,_xlpm.a + _xlpm.b)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -80,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="58">
   <si>
     <t>Result</t>
   </si>
@@ -251,6 +253,9 @@
   </si>
   <si>
     <t>Can I make a comment?</t>
+  </si>
+  <si>
+    <t>Apparently not</t>
   </si>
 </sst>
 </file>
@@ -407,10 +412,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,7 +1065,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="612" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="702" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1078,6 +1083,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1109,14 +1117,14 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -1429,14 +1437,14 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
@@ -2069,7 +2077,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2083,14 +2091,14 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="12"/>
+      <c r="H1" s="13"/>
       <c r="K1" s="5">
         <v>1</v>
       </c>
@@ -2381,7 +2389,7 @@
       </c>
       <c r="G20" s="11"/>
       <c r="H20" t="b" cm="1">
-        <f t="array" ref="H20:I32">E20:F32=G3:H15</f>
+        <f t="array" ref="H20:I32">FunctionOutput=Rubric</f>
         <v>1</v>
       </c>
       <c r="I20" t="b">
@@ -2420,6 +2428,9 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
+      <c r="K22" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.3">
       <c r="E23" s="6" t="str">
@@ -2465,7 +2476,7 @@
       <c r="I25" t="b">
         <v>1</v>
       </c>
-      <c r="K25" s="13" t="e" cm="1" vm="1">
+      <c r="K25" s="12" t="e" cm="1" vm="1">
         <f t="array" ref="K25">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, _xlpm.a + _xlpm.b)</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>